<commit_message>
Fixed numbering and dates
</commit_message>
<xml_diff>
--- a/CHECON.MECH.BOM.xlsx
+++ b/CHECON.MECH.BOM.xlsx
@@ -22,7 +22,7 @@
     <t>Tag:</t>
   </si>
   <si>
-    <t>CHECON.v1.1</t>
+    <t>CHECON.v1.3</t>
   </si>
   <si>
     <t>Product Number:</t>
@@ -169,8 +169,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -464,7 +465,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -498,13 +499,16 @@
     <xf numFmtId="1" fontId="5" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1868,7 +1872,7 @@
     <col min="3" max="3" width="51.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.75" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.0625" style="1" customWidth="1"/>
     <col min="7" max="7" width="17.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="43.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="99.125" style="1" customWidth="1"/>
@@ -1917,7 +1921,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="11">
-        <v>42010</v>
+        <v>42129</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
@@ -1937,7 +1941,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="11">
-        <v>42107</v>
+        <v>42129</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
@@ -1953,8 +1957,8 @@
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
@@ -1965,25 +1969,25 @@
       <c r="N4" s="13"/>
     </row>
     <row r="5" ht="18" customHeight="1">
-      <c r="A5" t="s" s="14">
+      <c r="A5" t="s" s="15">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="15">
+      <c r="B5" t="s" s="16">
         <v>9</v>
       </c>
-      <c r="C5" t="s" s="15">
+      <c r="C5" t="s" s="16">
         <v>10</v>
       </c>
-      <c r="D5" t="s" s="15">
+      <c r="D5" t="s" s="16">
         <v>11</v>
       </c>
-      <c r="E5" t="s" s="15">
+      <c r="E5" t="s" s="16">
         <v>12</v>
       </c>
-      <c r="F5" t="s" s="15">
+      <c r="F5" t="s" s="16">
         <v>13</v>
       </c>
-      <c r="G5" t="s" s="15">
+      <c r="G5" t="s" s="16">
         <v>14</v>
       </c>
       <c r="H5" t="s" s="8">
@@ -1992,797 +1996,797 @@
       <c r="I5" t="s" s="8">
         <v>16</v>
       </c>
-      <c r="J5" s="11"/>
+      <c r="J5" s="14"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="13"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="22"/>
+      <c r="A7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="20">
+      <c r="A9" s="21">
         <v>1</v>
       </c>
-      <c r="B9" t="s" s="23">
+      <c r="B9" t="s" s="24">
         <v>17</v>
       </c>
-      <c r="C9" t="s" s="24">
+      <c r="C9" t="s" s="25">
         <v>18</v>
       </c>
-      <c r="D9" t="s" s="23">
+      <c r="D9" t="s" s="24">
         <v>19</v>
       </c>
-      <c r="E9" t="s" s="24">
+      <c r="E9" t="s" s="25">
         <v>20</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" t="s" s="24">
+      <c r="F9" s="20"/>
+      <c r="G9" t="s" s="25">
         <v>21</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="19">
+      <c r="A11" s="20">
         <v>1</v>
       </c>
-      <c r="B11" t="s" s="23">
+      <c r="B11" t="s" s="24">
         <v>22</v>
       </c>
-      <c r="C11" t="s" s="23">
+      <c r="C11" t="s" s="24">
         <v>23</v>
       </c>
-      <c r="D11" t="s" s="23">
+      <c r="D11" t="s" s="24">
         <v>24</v>
       </c>
-      <c r="E11" t="s" s="24">
+      <c r="E11" t="s" s="25">
         <v>20</v>
       </c>
-      <c r="F11" s="19"/>
-      <c r="G11" t="s" s="23">
+      <c r="F11" s="20"/>
+      <c r="G11" t="s" s="24">
         <v>25</v>
       </c>
-      <c r="H11" s="19"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="20"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="20">
+      <c r="A13" s="21">
         <v>1</v>
       </c>
-      <c r="B13" t="s" s="24">
+      <c r="B13" t="s" s="25">
         <v>26</v>
       </c>
-      <c r="C13" t="s" s="24">
+      <c r="C13" t="s" s="25">
         <v>27</v>
       </c>
-      <c r="D13" t="s" s="23">
+      <c r="D13" t="s" s="24">
         <v>28</v>
       </c>
-      <c r="E13" t="s" s="24">
+      <c r="E13" t="s" s="25">
         <v>29</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" t="s" s="23">
+      <c r="F13" s="20"/>
+      <c r="G13" t="s" s="24">
         <v>25</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
     </row>
     <row r="15" ht="30" customHeight="1">
-      <c r="A15" s="20">
+      <c r="A15" s="21">
         <v>1</v>
       </c>
-      <c r="B15" t="s" s="24">
+      <c r="B15" t="s" s="25">
         <v>30</v>
       </c>
-      <c r="C15" t="s" s="24">
+      <c r="C15" t="s" s="25">
         <v>31</v>
       </c>
-      <c r="D15" t="s" s="26">
+      <c r="D15" t="s" s="27">
         <v>32</v>
       </c>
-      <c r="E15" t="s" s="24">
+      <c r="E15" t="s" s="25">
         <v>29</v>
       </c>
-      <c r="F15" s="19"/>
-      <c r="G15" t="s" s="24">
+      <c r="F15" s="20"/>
+      <c r="G15" t="s" s="25">
         <v>21</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="19">
+      <c r="A17" s="20">
         <v>1</v>
       </c>
-      <c r="B17" t="s" s="23">
+      <c r="B17" t="s" s="24">
         <v>33</v>
       </c>
-      <c r="C17" t="s" s="23">
+      <c r="C17" t="s" s="24">
         <v>34</v>
       </c>
-      <c r="D17" t="s" s="23">
+      <c r="D17" t="s" s="24">
         <v>35</v>
       </c>
-      <c r="E17" t="s" s="24">
+      <c r="E17" t="s" s="25">
         <v>29</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" t="s" s="24">
+      <c r="F17" s="20"/>
+      <c r="G17" t="s" s="25">
         <v>21</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
     </row>
     <row r="18" ht="17.25" customHeight="1">
-      <c r="A18" s="20"/>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="21"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
     </row>
     <row r="19" ht="19.5" customHeight="1">
-      <c r="A19" s="20">
+      <c r="A19" s="21">
         <v>1</v>
       </c>
-      <c r="B19" t="s" s="24">
+      <c r="B19" t="s" s="25">
         <v>36</v>
       </c>
-      <c r="C19" t="s" s="24">
+      <c r="C19" t="s" s="25">
         <v>37</v>
       </c>
-      <c r="D19" t="s" s="24">
+      <c r="D19" t="s" s="25">
         <v>38</v>
       </c>
-      <c r="E19" t="s" s="24">
+      <c r="E19" t="s" s="25">
         <v>29</v>
       </c>
-      <c r="F19" s="19"/>
-      <c r="G19" t="s" s="24">
+      <c r="F19" s="20"/>
+      <c r="G19" t="s" s="25">
         <v>21</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
     </row>
     <row r="20" ht="19.5" customHeight="1">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
     </row>
     <row r="21" ht="21" customHeight="1">
-      <c r="A21" s="20">
+      <c r="A21" s="21">
         <v>1</v>
       </c>
-      <c r="B21" t="s" s="24">
+      <c r="B21" t="s" s="25">
         <v>39</v>
       </c>
-      <c r="C21" t="s" s="24">
+      <c r="C21" t="s" s="25">
         <v>40</v>
       </c>
-      <c r="D21" t="s" s="24">
+      <c r="D21" t="s" s="25">
         <v>41</v>
       </c>
-      <c r="E21" t="s" s="24">
+      <c r="E21" t="s" s="25">
         <v>20</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" t="s" s="24">
+      <c r="F21" s="20"/>
+      <c r="G21" t="s" s="25">
         <v>21</v>
       </c>
-      <c r="H21" s="19"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
     </row>
     <row r="22" ht="30" customHeight="1">
-      <c r="A22" s="20">
+      <c r="A22" s="21">
         <v>2</v>
       </c>
-      <c r="B22" t="s" s="24">
+      <c r="B22" t="s" s="25">
         <v>42</v>
       </c>
-      <c r="C22" t="s" s="24">
+      <c r="C22" t="s" s="25">
         <v>43</v>
       </c>
-      <c r="D22" t="s" s="28">
+      <c r="D22" t="s" s="29">
         <v>44</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="19"/>
-      <c r="G22" t="s" s="24">
+      <c r="E22" s="21"/>
+      <c r="F22" s="20"/>
+      <c r="G22" t="s" s="25">
         <v>45</v>
       </c>
-      <c r="H22" t="s" s="23">
+      <c r="H22" t="s" s="24">
         <v>46</v>
       </c>
-      <c r="I22" s="25"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
+      <c r="I22" s="26"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
     </row>
     <row r="23" ht="30" customHeight="1">
-      <c r="A23" s="20"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="21"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
+      <c r="A23" s="21"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
     </row>
     <row r="24" ht="30" customHeight="1">
-      <c r="A24" s="20"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
     </row>
     <row r="25" ht="27" customHeight="1">
-      <c r="A25" s="20"/>
-      <c r="B25" s="29"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
+      <c r="A25" s="21"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="26"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
     </row>
     <row r="26" ht="27" customHeight="1">
-      <c r="A26" s="20"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="21"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="22"/>
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
     </row>
     <row r="27" ht="27" customHeight="1">
-      <c r="A27" s="20"/>
-      <c r="B27" s="29"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="25"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="22"/>
-      <c r="M27" s="22"/>
-      <c r="N27" s="22"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
     </row>
     <row r="28" ht="27" customHeight="1">
-      <c r="A28" s="20"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="21"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="22"/>
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
     </row>
     <row r="29" ht="27" customHeight="1">
-      <c r="A29" s="20"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="21"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="22"/>
-      <c r="M29" s="22"/>
-      <c r="N29" s="22"/>
+      <c r="A29" s="21"/>
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
     </row>
     <row r="30" ht="27" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="22"/>
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
     </row>
     <row r="31" ht="27" customHeight="1">
-      <c r="A31" s="20"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
+      <c r="A31" s="21"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
     </row>
     <row r="32" ht="27" customHeight="1">
-      <c r="A32" s="20"/>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="21"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="22"/>
-      <c r="M32" s="22"/>
-      <c r="N32" s="22"/>
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
     </row>
     <row r="33" ht="27" customHeight="1">
-      <c r="A33" s="20"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-      <c r="M33" s="22"/>
-      <c r="N33" s="22"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
     </row>
     <row r="34" ht="27" customHeight="1">
-      <c r="A34" s="20"/>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="21"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="22"/>
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
     </row>
     <row r="35" ht="27" customHeight="1">
-      <c r="A35" s="20"/>
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22"/>
-      <c r="N35" s="22"/>
+      <c r="A35" s="21"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
     </row>
     <row r="36" ht="27" customHeight="1">
-      <c r="A36" s="34"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="21"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="22"/>
-      <c r="M36" s="22"/>
-      <c r="N36" s="22"/>
+      <c r="A36" s="35"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="23"/>
+      <c r="L36" s="23"/>
+      <c r="M36" s="23"/>
+      <c r="N36" s="23"/>
     </row>
     <row r="37" ht="27" customHeight="1">
-      <c r="A37" s="35"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="37"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="22"/>
-      <c r="M37" s="22"/>
-      <c r="N37" s="22"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="37"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="36"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="23"/>
+      <c r="L37" s="23"/>
+      <c r="M37" s="23"/>
+      <c r="N37" s="23"/>
     </row>
     <row r="38" ht="27" customHeight="1">
-      <c r="A38" s="41"/>
-      <c r="B38" s="38"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="19"/>
-      <c r="H38" s="43"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="22"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="42"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="44"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="23"/>
+      <c r="L38" s="23"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
     </row>
     <row r="39" ht="27" customHeight="1">
-      <c r="A39" s="35"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="39"/>
-      <c r="I39" s="40"/>
-      <c r="J39" s="21"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="22"/>
-      <c r="M39" s="22"/>
-      <c r="N39" s="22"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="37"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="23"/>
+      <c r="L39" s="23"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
     </row>
     <row r="40" ht="27" customHeight="1">
-      <c r="A40" s="45"/>
-      <c r="B40" s="45"/>
-      <c r="C40" s="45"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="19"/>
-      <c r="H40" s="19"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="22"/>
-      <c r="M40" s="22"/>
-      <c r="N40" s="22"/>
+      <c r="A40" s="46"/>
+      <c r="B40" s="46"/>
+      <c r="C40" s="46"/>
+      <c r="D40" s="46"/>
+      <c r="E40" s="46"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="22"/>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
     </row>
     <row r="41" ht="30" customHeight="1">
-      <c r="A41" s="20"/>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="22"/>
-      <c r="M41" s="22"/>
-      <c r="N41" s="22"/>
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="22"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
     </row>
     <row r="42" ht="30" customHeight="1">
-      <c r="A42" s="20"/>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="22"/>
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
     </row>
     <row r="43" ht="45" customHeight="1">
-      <c r="A43" s="20"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="46"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="19"/>
-      <c r="H43" s="19"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="21"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="22"/>
-      <c r="M43" s="22"/>
-      <c r="N43" s="22"/>
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="47"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="23"/>
+      <c r="L43" s="23"/>
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
     </row>
     <row r="44" ht="45" customHeight="1">
-      <c r="A44" s="20"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="46"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="21"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="22"/>
-      <c r="M44" s="22"/>
-      <c r="N44" s="22"/>
+      <c r="A44" s="21"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="47"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="28"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="23"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="23"/>
+      <c r="N44" s="23"/>
     </row>
     <row r="45" ht="45" customHeight="1">
-      <c r="A45" s="20"/>
-      <c r="B45" s="20"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="46"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="21"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="22"/>
-      <c r="M45" s="22"/>
-      <c r="N45" s="22"/>
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="22"/>
+      <c r="K45" s="23"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
     </row>
     <row r="46" ht="30" customHeight="1">
-      <c r="A46" s="20"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="21"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="22"/>
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="22"/>
+      <c r="K46" s="23"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="25"/>
-      <c r="B47" s="19"/>
-      <c r="C47" s="19"/>
-      <c r="D47" s="19"/>
-      <c r="E47" s="19"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="21"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="22"/>
+      <c r="A47" s="26"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="23"/>
+      <c r="N47" s="23"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="25"/>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" t="s" s="23">
+      <c r="A48" s="26"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" t="s" s="24">
         <v>47</v>
       </c>
-      <c r="E48" s="19"/>
-      <c r="F48" s="19"/>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="21"/>
-      <c r="L48" s="21"/>
-      <c r="M48" s="22"/>
-      <c r="N48" s="22"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="22"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="23"/>
+      <c r="N48" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Edits to CHECON.MECH.ECO (copied commit messages) and CHECON.MECH.BOM (release tag and minor edit)
</commit_message>
<xml_diff>
--- a/CHECON.MECH.BOM.xlsx
+++ b/CHECON.MECH.BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,13 +20,13 @@
     <t>Product Name:</t>
   </si>
   <si>
-    <t>CHE Controller Mechanicals (VER 1.2 REV C)</t>
+    <t>CHE Controller Mechanicals </t>
   </si>
   <si>
     <t>Tag:</t>
   </si>
   <si>
-    <t>CHECON.MECH.v1.4 RC</t>
+    <t>CHECON.MECH.v1.4</t>
   </si>
   <si>
     <t>Product Number:</t>
@@ -463,8 +463,8 @@
   </sheetPr>
   <dimension ref="1:65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -474,7 +474,7 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="51.7555555555556"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.7555555555556"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.0444444444444"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.2666666666667"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="17.5"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="43.5037037037037"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="99.1222222222222"/>
@@ -12731,7 +12731,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.5"/>
-  <pageSetup paperSize="1" scale="45" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter>&amp;L&amp;"Arial,Regular"	&amp;P</oddFooter>

</xml_diff>

<commit_message>
Final edit to BOM - date correction
</commit_message>
<xml_diff>
--- a/CHECON.MECH.BOM.xlsx
+++ b/CHECON.MECH.BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -464,7 +464,7 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G30" activeCellId="0" sqref="G30"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1530,7 +1530,7 @@
         <v>6</v>
       </c>
       <c r="F2" s="8" t="n">
-        <v>42201</v>
+        <v>42213</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -2560,7 +2560,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="8" t="n">
-        <v>42201</v>
+        <v>42213</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>

</xml_diff>

<commit_message>
CHECON.MECH v1.5: Copied CHECON.TRAY v1.0 REV A and CHECON.CORETOP v1.0 REV A folders back into directory, deleted CHECON.CLIP v1.0 REV A folder
CHECON.MECH v1.5 (Happy Antenna) reverts the CHECON.CORETOP and
CHECON.TRAY parts, uses the revised *.COREMID and *.COREBOT parts.
</commit_message>
<xml_diff>
--- a/CHECON.MECH.BOM.xlsx
+++ b/CHECON.MECH.BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -464,7 +464,7 @@
   <dimension ref="1:65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12119,7 +12119,7 @@
     </row>
     <row r="14" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="18" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>30</v>

</xml_diff>